<commit_message>
fix show ui group by classes
</commit_message>
<xml_diff>
--- a/import/List_sv.xlsx
+++ b/import/List_sv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06433477-B763-4AC0-BA09-980BB1E561F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2EF643-44B1-4D13-B06A-2E7BE67379F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C17C6640-84FD-4348-8EF2-E5CA53A8DBEB}"/>
   </bookViews>
@@ -494,13 +494,13 @@
     <t>21211TT3805</t>
   </si>
   <si>
-    <t>21211TT2984</t>
-  </si>
-  <si>
     <t>22211TT1234</t>
   </si>
   <si>
     <t>23211TT1234</t>
+  </si>
+  <si>
+    <t>23211TT2984</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1039,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="45" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>68</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="46" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>34</v>

</xml_diff>